<commit_message>
Extraccion de contenido visiable para el usuario del codigo de la pagina
</commit_message>
<xml_diff>
--- a/Web-Scrapi/excelResultProfundo/0.0.urls_extraidas copy.xlsx
+++ b/Web-Scrapi/excelResultProfundo/0.0.urls_extraidas copy.xlsx
@@ -19,13 +19,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://web.archive.org/web/20160120015142/https://ssd.eff.org/en/module/how-use-otr-windows"&gt;«How</t>
+    <t>http://www.w3.org/1999/xlink\"</t>
   </si>
   <si>
     <t>https://uk.wikipedia.org/wiki/%D0%9D%D0%B0%D1%81%D0%BA%D1%80%D1%96%D0%B7%D0%BD%D0%B5_%D1%88%D0%B8%D1%84%D1%80%D1%83%D0%B2%D0%B0%D0%BD%D0%BD%D1%8F"</t>
   </si>
   <si>
-    <t>http://www.w3.org/1999/xlink\"</t>
+    <t>https://web.archive.org/web/20160120015142/https://ssd.eff.org/en/module/how-use-otr-windows"&gt;«How</t>
   </si>
   <si>
     <t/>
@@ -426,7 +426,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="127.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="145.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">

</xml_diff>